<commit_message>
Optiminzacion y ajustes de CtrlStr asi como algunos detallitos en EstructuraCtrl
</commit_message>
<xml_diff>
--- a/Documentacion/Controladores.xlsx
+++ b/Documentacion/Controladores.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="149">
   <si>
     <t>controlador</t>
   </si>
@@ -44,15 +45,12 @@
     <t>bajaUsuario</t>
   </si>
   <si>
-    <t>usuario </t>
+    <t>usuario</t>
   </si>
   <si>
     <t>consultaUsuario</t>
   </si>
   <si>
-    <t>usuario</t>
-  </si>
-  <si>
     <t>consultaUsuarios</t>
   </si>
   <si>
@@ -104,7 +102,7 @@
     <t>usuario,correo</t>
   </si>
   <si>
-    <t> -</t>
+    <t>-</t>
   </si>
   <si>
     <t>o</t>
@@ -131,7 +129,7 @@
     <t>bajaMaestro</t>
   </si>
   <si>
-    <t>codigo </t>
+    <t>codigo</t>
   </si>
   <si>
     <t>consultaMaestro</t>
@@ -161,6 +159,9 @@
     <t>codigo,nombramiento,temporal o definitivo</t>
   </si>
   <si>
+    <t>FUNCION DE CLONAR</t>
+  </si>
+  <si>
     <t>ESTRUCTURA (2)</t>
   </si>
   <si>
@@ -260,7 +261,7 @@
     <t>consultaEvidencia</t>
   </si>
   <si>
-    <t>curso </t>
+    <t>curso</t>
   </si>
   <si>
     <t>consultaEvidencias</t>
@@ -281,7 +282,7 @@
     <t>consultaObservaciones</t>
   </si>
   <si>
-    <t>evidencia </t>
+    <t>evidencia</t>
   </si>
   <si>
     <t>ASISTENCIAS (5)</t>
@@ -414,6 +415,54 @@
   </si>
   <si>
     <t>modificacionSuple</t>
+  </si>
+  <si>
+    <t>primario</t>
+  </si>
+  <si>
+    <t>quien</t>
+  </si>
+  <si>
+    <t>secundario</t>
+  </si>
+  <si>
+    <t>terciario</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>AltaUsuario</t>
+  </si>
+  <si>
+    <t>ConsultaUsuarios</t>
+  </si>
+  <si>
+    <t>ModificarUsuario(MiUsuario)</t>
+  </si>
+  <si>
+    <t>consultaUsuario(MiUsuario)</t>
+  </si>
+  <si>
+    <t>Estructura</t>
+  </si>
+  <si>
+    <t>Departamentos</t>
+  </si>
+  <si>
+    <t>AltaDepartamento</t>
+  </si>
+  <si>
+    <t>consultaDepartamentoPertenencia</t>
+  </si>
+  <si>
+    <t>Carreras</t>
+  </si>
+  <si>
+    <t>Academias</t>
+  </si>
+  <si>
+    <t>Materias</t>
   </si>
 </sst>
 </file>
@@ -455,7 +504,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +515,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -566,7 +621,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -631,6 +686,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -646,13 +713,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -660,14 +727,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5714285714286"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2857142857143"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.8571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.280612244898"/>
+    <col collapsed="false" hidden="true" max="5" min="4" style="1" width="0"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="0" width="10.7295918367347"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.7295918367347"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -699,7 +765,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="8" t="s">
         <v>8</v>
@@ -712,7 +778,7 @@
       </c>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
@@ -721,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="9"/>
       <c r="I4" s="10" t="s">
@@ -729,209 +795,213 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="9"/>
       <c r="I5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="9"/>
       <c r="I6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="9"/>
       <c r="I7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="9"/>
       <c r="I8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="9"/>
       <c r="I9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="E10" s="14"/>
       <c r="I10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="E11" s="7"/>
       <c r="I11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="9"/>
       <c r="I13" s="15"/>
       <c r="J13" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="14"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
@@ -941,7 +1011,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>50</v>
@@ -954,7 +1024,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>52</v>
@@ -967,7 +1037,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>52</v>
@@ -980,20 +1050,20 @@
         <v>54</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>52</v>
@@ -1006,7 +1076,7 @@
         <v>56</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>57</v>
@@ -1022,7 +1092,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>59</v>
@@ -1038,7 +1108,7 @@
         <v>61</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>59</v>
@@ -1054,10 +1124,10 @@
         <v>63</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="9"/>
     </row>
@@ -1067,7 +1137,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>57</v>
@@ -1080,7 +1150,7 @@
         <v>65</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>66</v>
@@ -1093,7 +1163,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>59</v>
@@ -1106,7 +1176,7 @@
         <v>68</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>59</v>
@@ -1119,10 +1189,10 @@
         <v>69</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="9"/>
     </row>
@@ -1132,7 +1202,7 @@
         <v>70</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>66</v>
@@ -1145,7 +1215,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>72</v>
@@ -1158,7 +1228,7 @@
         <v>73</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>59</v>
@@ -1171,7 +1241,7 @@
         <v>74</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>59</v>
@@ -1184,10 +1254,10 @@
         <v>75</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="9"/>
     </row>
@@ -1197,7 +1267,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>72</v>
@@ -1225,7 +1295,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>81</v>
@@ -1238,10 +1308,10 @@
         <v>82</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E39" s="9"/>
     </row>
@@ -1277,7 +1347,7 @@
         <v>87</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>88</v>
@@ -1292,7 +1362,7 @@
         <v>90</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>91</v>
@@ -1305,7 +1375,7 @@
         <v>92</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>93</v>
@@ -1357,7 +1427,7 @@
         <v>99</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>93</v>
@@ -1370,7 +1440,7 @@
         <v>100</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>101</v>
@@ -1383,7 +1453,7 @@
         <v>102</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>103</v>
@@ -1396,7 +1466,7 @@
         <v>104</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>103</v>
@@ -1409,10 +1479,10 @@
         <v>105</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E52" s="9"/>
     </row>
@@ -1422,7 +1492,7 @@
         <v>106</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D53" s="13" t="s">
         <v>103</v>
@@ -1437,7 +1507,7 @@
         <v>108</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7"/>
@@ -1448,7 +1518,7 @@
         <v>109</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
@@ -1459,7 +1529,7 @@
         <v>110</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
@@ -1470,7 +1540,7 @@
         <v>111</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
@@ -1481,7 +1551,7 @@
         <v>112</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
@@ -1492,7 +1562,7 @@
         <v>113</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
@@ -1503,7 +1573,7 @@
         <v>114</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
@@ -1514,7 +1584,7 @@
         <v>115</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
@@ -1525,7 +1595,7 @@
         <v>116</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="9"/>
@@ -1536,7 +1606,7 @@
         <v>117</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
@@ -1547,7 +1617,7 @@
         <v>118</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="9"/>
@@ -1558,7 +1628,7 @@
         <v>119</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
@@ -1569,7 +1639,7 @@
         <v>120</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="9"/>
@@ -1580,7 +1650,7 @@
         <v>121</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="14"/>
@@ -1593,7 +1663,7 @@
         <v>123</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="7"/>
@@ -1604,7 +1674,7 @@
         <v>124</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
@@ -1615,7 +1685,7 @@
         <v>125</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="9"/>
@@ -1626,7 +1696,7 @@
         <v>126</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
@@ -1637,7 +1707,7 @@
         <v>127</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="9"/>
@@ -1648,7 +1718,7 @@
         <v>128</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
@@ -1659,7 +1729,7 @@
         <v>129</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
@@ -1670,7 +1740,7 @@
         <v>130</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
@@ -1681,7 +1751,7 @@
         <v>131</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
@@ -1692,7 +1762,7 @@
         <v>132</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="14"/>
@@ -1717,4 +1787,223 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="6.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="26.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="6.6530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="32.1836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="6.6530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0"/>
+      <c r="I3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0"/>
+      <c r="I4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0"/>
+      <c r="I5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18"/>
+      <c r="C7" s="0"/>
+      <c r="E7" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18"/>
+      <c r="C8" s="0"/>
+      <c r="E8" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0"/>
+      <c r="E9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A6:A8"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>